<commit_message>
updated tables and figures
</commit_message>
<xml_diff>
--- a/tables/Table5_ram_ms_fisheries_overview.xlsx
+++ b/tables/Table5_ram_ms_fisheries_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/mscom/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1FCD71C9-9CF1-4841-8234-8422DF3939C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26254E21-A73F-0B4F-95AB-5D3596F15192}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table5_ram_ms_fisheries_overvie" sheetId="1" r:id="rId1"/>
@@ -20,28 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Australia SESSF</t>
-  </si>
-  <si>
-    <t>NZ Chatham Rise</t>
-  </si>
-  <si>
-    <t>US BSAI groundfish</t>
-  </si>
-  <si>
-    <t>US GB groundfish</t>
-  </si>
-  <si>
-    <t>US GB/GOM groundfish</t>
-  </si>
-  <si>
-    <t>US GOM groundfish</t>
-  </si>
-  <si>
-    <t>US West Coast DTS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Fishery</t>
   </si>
@@ -70,16 +49,100 @@
     <t>3 - pacific cod, walleye pollock, walleye pollock, yellowfin sole</t>
   </si>
   <si>
-    <t># of years of catch data</t>
-  </si>
-  <si>
-    <t>Mean correlation in effort time series</t>
+    <t>ICCAT South Atlantic tunas</t>
+  </si>
+  <si>
+    <t>2 - albacore tuna, swordfish</t>
+  </si>
+  <si>
+    <t>IOTC Indian Ocean tunas</t>
+  </si>
+  <si>
+    <t>4 - albacore tuna, bigeye tuna, black marlin, indo-pacific blue marlin, skipjack tuna, striped marlin, swordfish, yellowfin tuna</t>
+  </si>
+  <si>
+    <t>SPC West Pacific tunas</t>
+  </si>
+  <si>
+    <t>4 - bigeye tuna, skipjack tuna, striped marlin, yellowfin tuna</t>
+  </si>
+  <si>
+    <t>ICCAT Atlantic tunas</t>
+  </si>
+  <si>
+    <t>2 - sailfish, yellowfin tuna</t>
+  </si>
+  <si>
+    <t>Australia SE scalefish/sharks</t>
+  </si>
+  <si>
+    <t>ICCAT East Atlantic tunas</t>
+  </si>
+  <si>
+    <t>5 - atlantic bluefin tuna, bigeye tuna, blue marlin, skipjack tuna, swordfish, white marlin</t>
+  </si>
+  <si>
+    <t>ICCAT West Atlantic tunas</t>
+  </si>
+  <si>
+    <t>2 - atlantic bluefin tuna, sailfish, skipjack tuna</t>
+  </si>
+  <si>
+    <t>IATTC East Pacific tunas</t>
+  </si>
+  <si>
+    <t>2 - bigeye tuna, skipjack tuna, striped marlin, swordfish, yellowfin tuna</t>
+  </si>
+  <si>
+    <t>USA West Coast DTS</t>
+  </si>
+  <si>
+    <t>NZ Chatham Rise middle-depth</t>
+  </si>
+  <si>
+    <t>USA GB groundfish</t>
+  </si>
+  <si>
+    <t>USA GB/GOM groundfish</t>
+  </si>
+  <si>
+    <t>ICCAT Mediterranean tunas</t>
+  </si>
+  <si>
+    <t>ISC North Pacific tunas</t>
+  </si>
+  <si>
+    <t>2 - albacore tuna, blue shark, blue marlin, swordfish</t>
+  </si>
+  <si>
+    <t>USA GOM groundfish</t>
+  </si>
+  <si>
+    <t>USA BSAI groundfish</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>of ER data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -397,7 +460,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -518,6 +581,13 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -568,9 +638,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -926,132 +999,322 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E19" sqref="A2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
-      </c>
-      <c r="C3">
-        <v>47</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.57516171347513501</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1">
-        <v>0.42799991342441701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.83346108975113198</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.7099416920561601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.81120765234287096</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.2803359415712698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.80397813668933804</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.2820396292148901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.76406817679156702</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.75378860015121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
         <v>28</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.42310467186475098</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
+      <c r="D8" s="1">
+        <v>0.70382731389724695</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.13577943969206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.67886222421873799</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.6297648599711501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>51</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.57335199057975506</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.54866684097692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
         <v>35</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.27489561180405803</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D11" s="1">
+        <v>0.51314165290787905</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.4316652866480799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.47670325734810998</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.9764811653101999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
+      <c r="C13">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.40508100073693398</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1.8335625285708099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.29232976494715901</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.40604606262889</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.234163580073599</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.4852747377018301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.74152883838989E-4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1.0005194488152001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.26964963799935898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-2.17208968963752E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-1.1642489110762399E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.99894615324264402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-3.5558860958535103E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.0355782724841001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
         <v>36</v>
       </c>
-      <c r="D9" s="1">
-        <v>-0.14325028272565199</v>
+      <c r="D19" s="1">
+        <v>-0.13955376018917001</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.85683224936067703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>